<commit_message>
impact of data preprocessing and augmentation done
</commit_message>
<xml_diff>
--- a/error/pp_and_da/pp_and_da.xlsx
+++ b/error/pp_and_da/pp_and_da.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Classe</t>
   </si>
@@ -42,13 +42,7 @@
     <t>Mínimo</t>
   </si>
   <si>
-    <t>64x64</t>
-  </si>
-  <si>
     <t>80x80</t>
-  </si>
-  <si>
-    <t>Classe\Side</t>
   </si>
   <si>
     <t>96x96</t>
@@ -70,6 +64,9 @@
   </si>
   <si>
     <t>pp + flips + rot</t>
+  </si>
+  <si>
+    <t>Class\Opt</t>
   </si>
 </sst>
 </file>
@@ -149,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -169,6 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,25 +513,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.84656461374154501</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.71306514773940899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -608,25 +606,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.82342470630117481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.99964400142399434</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -701,25 +699,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.86187255250979</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.83980064079743677</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.99964400142399434</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -728,289 +726,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-D39A-4E85-82AF-F0A123758A1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tamanho!$S$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>80</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tamanho!$M$3:$M$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tamanho!$S$3:$S$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D39A-4E85-82AF-F0A123758A1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tamanho!$T$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>96</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tamanho!$M$3:$M$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tamanho!$T$3:$T$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D39A-4E85-82AF-F0A123758A1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tamanho!$U$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tamanho!$M$3:$M$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tamanho!$U$3:$U$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D39A-4E85-82AF-F0A123758A1F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1025,6 +740,353 @@
         <c:smooth val="0"/>
         <c:axId val="317254856"/>
         <c:axId val="317249936"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$S$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>80</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$M$3:$M$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$S$3:$S$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-D39A-4E85-82AF-F0A123758A1F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="6"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$T$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>96</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$M$3:$M$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$T$3:$T$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000006-D39A-4E85-82AF-F0A123758A1F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="7"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$U$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>128</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$M$3:$M$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tamanho!$U$3:$U$9</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-D39A-4E85-82AF-F0A123758A1F}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="317254856"/>
@@ -1377,7 +1439,9 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2003,11 +2067,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.0194</cdr:x>
-      <cdr:y>0.65933</cdr:y>
+      <cdr:y>0.82809</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.98547</cdr:x>
-      <cdr:y>0.6861</cdr:y>
+      <cdr:y>0.85486</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2022,7 +2086,7 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="216539" y="4316717"/>
+          <a:off x="216539" y="5421617"/>
           <a:ext cx="10784529" cy="175266"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -2328,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
+      <selection activeCell="AF29" sqref="AF29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2341,7 +2405,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2402,22 +2466,22 @@
         <v>1</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="S2" s="8">
         <v>80</v>
@@ -2471,17 +2535,17 @@
         <f>K11</f>
         <v>0.73406906372374514</v>
       </c>
-      <c r="P3" t="e">
+      <c r="P3">
         <f>K20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q3" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <f>K29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R3" t="e">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <f>K38</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S3" t="e">
         <f>K47</f>
@@ -2538,17 +2602,17 @@
         <f t="shared" ref="O4:O9" si="1">K12</f>
         <v>0.10964756140975436</v>
       </c>
-      <c r="P4" t="e">
+      <c r="P4">
         <f t="shared" ref="P4:P9" si="2">K21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <f t="shared" ref="Q4:Q9" si="3">K30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" t="e">
+        <v>1</v>
+      </c>
+      <c r="R4">
         <f t="shared" ref="R4:R9" si="4">K39</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S4" t="e">
         <f t="shared" ref="S4:S9" si="5">K48</f>
@@ -2605,17 +2669,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P5" t="e">
+      <c r="P5">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" t="e">
+        <v>0.84656461374154501</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" t="e">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.86187255250979</v>
       </c>
       <c r="S5" t="e">
         <f t="shared" si="5"/>
@@ -2672,17 +2736,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P6" t="e">
+      <c r="P6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q6" t="e">
+        <v>0.71306514773940899</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R6" t="e">
+        <v>0.82342470630117481</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.83980064079743677</v>
       </c>
       <c r="S6" t="e">
         <f t="shared" si="5"/>
@@ -2739,17 +2803,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P7" t="e">
+      <c r="P7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" t="e">
+        <v>0.99964400142399434</v>
+      </c>
+      <c r="R7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S7" t="e">
         <f t="shared" si="5"/>
@@ -2806,17 +2870,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P8" t="e">
+      <c r="P8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" t="e">
+        <v>1</v>
+      </c>
+      <c r="R8">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.99964400142399434</v>
       </c>
       <c r="S8" t="e">
         <f t="shared" si="5"/>
@@ -2844,17 +2908,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P9" t="e">
+      <c r="P9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" t="e">
+        <v>1</v>
+      </c>
+      <c r="R9">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S9" t="e">
         <f t="shared" si="5"/>
@@ -2872,7 +2936,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -2945,31 +3009,31 @@
       <c r="M11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="13">
         <f>AVERAGE(N3:N9)</f>
         <v>0.92107003000559418</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="10">
         <f>AVERAGE(O3:O9)</f>
         <v>0.40624523216192848</v>
       </c>
-      <c r="P11" t="e">
+      <c r="P11" s="10">
         <f t="shared" ref="P11:R11" si="8">AVERAGE(P3:P9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" t="e">
+        <v>0.93708996592585059</v>
+      </c>
+      <c r="Q11" s="10">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" t="e">
+        <v>0.97472410110359564</v>
+      </c>
+      <c r="R11" s="10">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0.95733102781874579</v>
       </c>
       <c r="S11" s="10" t="e">
         <f>AVERAGE(S3:S9)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T11" s="1" t="e">
+      <c r="T11" s="10" t="e">
         <f>AVERAGE(T3:T9)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3012,31 +3076,31 @@
       <c r="M12" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="13">
         <f>MEDIAN(N3:N9)</f>
         <v>0.99359202563189752</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="10">
         <f>MEDIAN(O3:O9)</f>
         <v>0.10964756140975436</v>
       </c>
-      <c r="P12" t="e">
+      <c r="P12" s="10">
         <f t="shared" ref="P12:T12" si="9">MEDIAN(P3:P9)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="10">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" t="e">
+        <v>1</v>
+      </c>
+      <c r="R12" s="10">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S12" s="10" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T12" s="1" t="e">
+      <c r="T12" s="10" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -3079,35 +3143,35 @@
       <c r="M13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="13">
         <f>LARGE(N3:N9,1)</f>
         <v>1</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="10">
         <f>LARGE(O3:O9,1)</f>
         <v>1</v>
       </c>
-      <c r="P13" t="e">
+      <c r="P13" s="10">
         <f t="shared" ref="P13:T13" si="10">LARGE(P3:P9,1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q13" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="10">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R13" s="1" t="e">
+        <v>1</v>
+      </c>
+      <c r="R13" s="10">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" s="1" t="e">
+        <v>1</v>
+      </c>
+      <c r="S13" s="10" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T13" s="1" t="e">
+      <c r="T13" s="10" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U13" s="1" t="e">
+      <c r="U13" s="10" t="e">
         <f t="shared" ref="U13" si="11">LARGE(U3:U9,1)</f>
         <v>#DIV/0!</v>
       </c>
@@ -3146,31 +3210,31 @@
       <c r="M14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="13">
         <f>SMALL(N3:N9,1)</f>
         <v>0.59166963332146671</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="10">
         <f>SMALL(O3:O9,1)</f>
         <v>0</v>
       </c>
-      <c r="P14" t="e">
+      <c r="P14" s="10">
         <f t="shared" ref="P14:T14" si="12">SMALL(P3:P9,1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q14" t="e">
+        <v>0.71306514773940899</v>
+      </c>
+      <c r="Q14" s="10">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R14" t="e">
+        <v>0.82342470630117481</v>
+      </c>
+      <c r="R14" s="10">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>0.83980064079743677</v>
       </c>
       <c r="S14" s="10" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T14" s="1" t="e">
+      <c r="T14" s="10" t="e">
         <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
@@ -3290,7 +3354,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>0</v>
@@ -3326,10 +3390,30 @@
       <c r="B20" s="2">
         <v>0</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="K20" s="3" t="e">
+      <c r="C20" s="7">
+        <v>2809</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
         <f>C20/SUM(C20:I20)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
@@ -3340,11 +3424,30 @@
       <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="K21" s="3" t="e">
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2809</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
         <f>D21/SUM(C21:I21)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="R21" s="9"/>
     </row>
@@ -3353,11 +3456,30 @@
       <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="E22" s="5"/>
-      <c r="K22" s="3" t="e">
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>2378</v>
+      </c>
+      <c r="F22">
+        <v>431</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
         <f>E22/SUM(C22:I22)</f>
-        <v>#DIV/0!</v>
+        <v>0.84656461374154501</v>
       </c>
       <c r="R22" s="9"/>
     </row>
@@ -3366,11 +3488,30 @@
       <c r="B23" s="2">
         <v>3</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="F23" s="5"/>
-      <c r="K23" s="3" t="e">
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>674</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>132</v>
+      </c>
+      <c r="K23" s="3">
         <f>F23/SUM(C23:I23)</f>
-        <v>#DIV/0!</v>
+        <v>0.71306514773940899</v>
       </c>
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
@@ -3381,11 +3522,30 @@
       <c r="B24" s="2">
         <v>4</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="G24" s="5"/>
-      <c r="K24" s="3" t="e">
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2809</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
         <f>G24/SUM(C24:I24)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="R24" s="9"/>
     </row>
@@ -3394,11 +3554,30 @@
       <c r="B25" s="2">
         <v>5</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="H25" s="5"/>
-      <c r="K25" s="3" t="e">
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2809</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
         <f>H25/SUM(C25:I25)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="R25" s="9"/>
     </row>
@@ -3407,16 +3586,35 @@
       <c r="B26" s="2">
         <v>6</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="I26" s="5"/>
-      <c r="K26" s="3" t="e">
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>2809</v>
+      </c>
+      <c r="K26" s="3">
         <f>I26/SUM(C26:I26)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
@@ -3451,10 +3649,30 @@
       <c r="B29" s="2">
         <v>0</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="K29" s="3" t="e">
+      <c r="C29" s="7">
+        <v>2809</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
         <f>C29/SUM(C29:I29)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M29" s="1"/>
       <c r="O29" s="1"/>
@@ -3464,11 +3682,30 @@
       <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
-      <c r="K30" s="3" t="e">
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2809</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
         <f>D30/SUM(C30:I30)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -3476,11 +3713,30 @@
       <c r="B31" s="2">
         <v>2</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="E31" s="5"/>
-      <c r="K31" s="3" t="e">
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>2809</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
         <f>E31/SUM(C31:I31)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -3488,11 +3744,30 @@
       <c r="B32" s="2">
         <v>3</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="F32" s="5"/>
-      <c r="K32" s="3" t="e">
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>496</v>
+      </c>
+      <c r="F32" s="5">
+        <v>2313</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
         <f>F32/SUM(C32:I32)</f>
-        <v>#DIV/0!</v>
+        <v>0.82342470630117481</v>
       </c>
       <c r="M32" s="1"/>
       <c r="O32" s="1"/>
@@ -3502,11 +3777,30 @@
       <c r="B33" s="2">
         <v>4</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="G33" s="5"/>
-      <c r="K33" s="3" t="e">
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2808</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
         <f>G33/SUM(C33:I33)</f>
-        <v>#DIV/0!</v>
+        <v>0.99964400142399434</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -3514,11 +3808,30 @@
       <c r="B34" s="2">
         <v>5</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="H34" s="5"/>
-      <c r="K34" s="3" t="e">
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>2809</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
         <f>H34/SUM(C34:I34)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -3526,16 +3839,35 @@
       <c r="B35" s="2">
         <v>6</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="I35" s="5"/>
-      <c r="K35" s="3" t="e">
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>2809</v>
+      </c>
+      <c r="K35" s="3">
         <f>I35/SUM(C35:I35)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
@@ -3570,10 +3902,30 @@
       <c r="B38" s="2">
         <v>0</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="K38" s="3" t="e">
+      <c r="C38" s="7">
+        <v>2809</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
         <f>C38/SUM(C38:I38)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M38" s="1"/>
       <c r="O38" s="1"/>
@@ -3583,11 +3935,30 @@
       <c r="B39" s="2">
         <v>1</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="5"/>
-      <c r="K39" s="3" t="e">
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2809</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
         <f>D39/SUM(C39:I39)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -3595,11 +3966,30 @@
       <c r="B40" s="2">
         <v>2</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="E40" s="5"/>
-      <c r="K40" s="3" t="e">
+      <c r="C40" s="6">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>379</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2421</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="K40" s="3">
         <f>E40/SUM(C40:I40)</f>
-        <v>#DIV/0!</v>
+        <v>0.86187255250979</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3607,11 +3997,30 @@
       <c r="B41" s="2">
         <v>3</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="F41" s="5"/>
-      <c r="K41" s="3" t="e">
+      <c r="C41" s="6">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>325</v>
+      </c>
+      <c r="E41">
+        <v>54</v>
+      </c>
+      <c r="F41" s="5">
+        <v>2359</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>71</v>
+      </c>
+      <c r="K41" s="3">
         <f>F41/SUM(C41:I41)</f>
-        <v>#DIV/0!</v>
+        <v>0.83980064079743677</v>
       </c>
       <c r="M41" s="1"/>
       <c r="O41" s="1"/>
@@ -3621,11 +4030,30 @@
       <c r="B42" s="2">
         <v>4</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="G42" s="5"/>
-      <c r="K42" s="3" t="e">
+      <c r="C42" s="6">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>2809</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
         <f>G42/SUM(C42:I42)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3633,11 +4061,30 @@
       <c r="B43" s="2">
         <v>5</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="H43" s="5"/>
-      <c r="K43" s="3" t="e">
+      <c r="C43" s="6">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>2808</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
         <f>H43/SUM(C43:I43)</f>
-        <v>#DIV/0!</v>
+        <v>0.99964400142399434</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -3645,16 +4092,35 @@
       <c r="B44" s="2">
         <v>6</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="I44" s="5"/>
-      <c r="K44" s="3" t="e">
+      <c r="C44" s="6">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>2809</v>
+      </c>
+      <c r="K44" s="3">
         <f>I44/SUM(C44:I44)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>0</v>
@@ -3689,7 +4155,27 @@
       <c r="B47" s="2">
         <v>0</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7">
+        <v>0</v>
+      </c>
+      <c r="D47" s="7">
+        <v>0</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0</v>
+      </c>
+      <c r="H47" s="7">
+        <v>0</v>
+      </c>
+      <c r="I47" s="7">
+        <v>0</v>
+      </c>
       <c r="K47" s="3" t="e">
         <f>C47/SUM(C47:I47)</f>
         <v>#DIV/0!</v>
@@ -3702,8 +4188,27 @@
       <c r="B48" s="2">
         <v>1</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="5"/>
+      <c r="C48" s="7">
+        <v>0</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0</v>
+      </c>
+      <c r="I48" s="7">
+        <v>0</v>
+      </c>
       <c r="K48" s="3" t="e">
         <f>D48/SUM(C48:I48)</f>
         <v>#DIV/0!</v>
@@ -3714,8 +4219,27 @@
       <c r="B49" s="2">
         <v>2</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="E49" s="5"/>
+      <c r="C49" s="7">
+        <v>0</v>
+      </c>
+      <c r="D49" s="7">
+        <v>0</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0</v>
+      </c>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
+      <c r="I49" s="7">
+        <v>0</v>
+      </c>
       <c r="K49" s="3" t="e">
         <f>E49/SUM(C49:I49)</f>
         <v>#DIV/0!</v>
@@ -3726,8 +4250,27 @@
       <c r="B50" s="2">
         <v>3</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="F50" s="5"/>
+      <c r="C50" s="7">
+        <v>0</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0</v>
+      </c>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
+      <c r="I50" s="7">
+        <v>0</v>
+      </c>
       <c r="K50" s="3" t="e">
         <f>F50/SUM(C50:I50)</f>
         <v>#DIV/0!</v>
@@ -3740,8 +4283,27 @@
       <c r="B51" s="2">
         <v>4</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="G51" s="5"/>
+      <c r="C51" s="7">
+        <v>0</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0</v>
+      </c>
       <c r="K51" s="3" t="e">
         <f>G51/SUM(C51:I51)</f>
         <v>#DIV/0!</v>
@@ -3752,8 +4314,27 @@
       <c r="B52" s="2">
         <v>5</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="H52" s="5"/>
+      <c r="C52" s="7">
+        <v>0</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0</v>
+      </c>
+      <c r="G52" s="7">
+        <v>0</v>
+      </c>
+      <c r="H52" s="7">
+        <v>0</v>
+      </c>
+      <c r="I52" s="7">
+        <v>0</v>
+      </c>
       <c r="K52" s="3" t="e">
         <f>H52/SUM(C52:I52)</f>
         <v>#DIV/0!</v>
@@ -3764,8 +4345,27 @@
       <c r="B53" s="2">
         <v>6</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="I53" s="5"/>
+      <c r="C53" s="7">
+        <v>0</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0</v>
+      </c>
+      <c r="H53" s="7">
+        <v>0</v>
+      </c>
+      <c r="I53" s="7">
+        <v>0</v>
+      </c>
       <c r="K53" s="3" t="e">
         <f>I53/SUM(C53:I53)</f>
         <v>#DIV/0!</v>
@@ -3773,7 +4373,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>0</v>
@@ -3808,7 +4408,27 @@
       <c r="B56" s="2">
         <v>0</v>
       </c>
-      <c r="C56" s="7"/>
+      <c r="C56" s="7">
+        <v>0</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7">
+        <v>0</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0</v>
+      </c>
+      <c r="H56" s="7">
+        <v>0</v>
+      </c>
+      <c r="I56" s="7">
+        <v>0</v>
+      </c>
       <c r="K56" s="3" t="e">
         <f>C56/SUM(C56:I56)</f>
         <v>#DIV/0!</v>
@@ -3821,8 +4441,27 @@
       <c r="B57" s="2">
         <v>1</v>
       </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="5"/>
+      <c r="C57" s="7">
+        <v>0</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0</v>
+      </c>
+      <c r="F57" s="7">
+        <v>0</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0</v>
+      </c>
+      <c r="H57" s="7">
+        <v>0</v>
+      </c>
+      <c r="I57" s="7">
+        <v>0</v>
+      </c>
       <c r="K57" s="3" t="e">
         <f>D57/SUM(C57:I57)</f>
         <v>#DIV/0!</v>
@@ -3833,8 +4472,27 @@
       <c r="B58" s="2">
         <v>2</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="E58" s="5"/>
+      <c r="C58" s="7">
+        <v>0</v>
+      </c>
+      <c r="D58" s="7">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0</v>
+      </c>
+      <c r="G58" s="7">
+        <v>0</v>
+      </c>
+      <c r="H58" s="7">
+        <v>0</v>
+      </c>
+      <c r="I58" s="7">
+        <v>0</v>
+      </c>
       <c r="K58" s="3" t="e">
         <f>E58/SUM(C58:I58)</f>
         <v>#DIV/0!</v>
@@ -3845,8 +4503,27 @@
       <c r="B59" s="2">
         <v>3</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="F59" s="5"/>
+      <c r="C59" s="7">
+        <v>0</v>
+      </c>
+      <c r="D59" s="7">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0</v>
+      </c>
+      <c r="G59" s="7">
+        <v>0</v>
+      </c>
+      <c r="H59" s="7">
+        <v>0</v>
+      </c>
+      <c r="I59" s="7">
+        <v>0</v>
+      </c>
       <c r="K59" s="3" t="e">
         <f>F59/SUM(C59:I59)</f>
         <v>#DIV/0!</v>
@@ -3859,8 +4536,27 @@
       <c r="B60" s="2">
         <v>4</v>
       </c>
-      <c r="C60" s="6"/>
-      <c r="G60" s="5"/>
+      <c r="C60" s="7">
+        <v>0</v>
+      </c>
+      <c r="D60" s="7">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0</v>
+      </c>
+      <c r="F60" s="7">
+        <v>0</v>
+      </c>
+      <c r="G60" s="7">
+        <v>0</v>
+      </c>
+      <c r="H60" s="7">
+        <v>0</v>
+      </c>
+      <c r="I60" s="7">
+        <v>0</v>
+      </c>
       <c r="K60" s="3" t="e">
         <f>G60/SUM(C60:I60)</f>
         <v>#DIV/0!</v>
@@ -3871,8 +4567,27 @@
       <c r="B61" s="2">
         <v>5</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="H61" s="5"/>
+      <c r="C61" s="7">
+        <v>0</v>
+      </c>
+      <c r="D61" s="7">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0</v>
+      </c>
+      <c r="G61" s="7">
+        <v>0</v>
+      </c>
+      <c r="H61" s="7">
+        <v>0</v>
+      </c>
+      <c r="I61" s="7">
+        <v>0</v>
+      </c>
       <c r="K61" s="3" t="e">
         <f>H61/SUM(C61:I61)</f>
         <v>#DIV/0!</v>
@@ -3883,8 +4598,27 @@
       <c r="B62" s="2">
         <v>6</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="I62" s="5"/>
+      <c r="C62" s="7">
+        <v>0</v>
+      </c>
+      <c r="D62" s="7">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0</v>
+      </c>
+      <c r="G62" s="7">
+        <v>0</v>
+      </c>
+      <c r="H62" s="7">
+        <v>0</v>
+      </c>
+      <c r="I62" s="7">
+        <v>0</v>
+      </c>
       <c r="K62" s="3" t="e">
         <f>I62/SUM(C62:I62)</f>
         <v>#DIV/0!</v>
@@ -3892,7 +4626,7 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>0</v>
@@ -3927,7 +4661,27 @@
       <c r="B65" s="2">
         <v>0</v>
       </c>
-      <c r="C65" s="7"/>
+      <c r="C65" s="7">
+        <v>0</v>
+      </c>
+      <c r="D65" s="7">
+        <v>0</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0</v>
+      </c>
+      <c r="G65" s="7">
+        <v>0</v>
+      </c>
+      <c r="H65" s="7">
+        <v>0</v>
+      </c>
+      <c r="I65" s="7">
+        <v>0</v>
+      </c>
       <c r="K65" s="3" t="e">
         <f>C65/SUM(C65:I65)</f>
         <v>#DIV/0!</v>
@@ -3940,8 +4694,27 @@
       <c r="B66" s="2">
         <v>1</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="5"/>
+      <c r="C66" s="7">
+        <v>0</v>
+      </c>
+      <c r="D66" s="7">
+        <v>0</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0</v>
+      </c>
+      <c r="G66" s="7">
+        <v>0</v>
+      </c>
+      <c r="H66" s="7">
+        <v>0</v>
+      </c>
+      <c r="I66" s="7">
+        <v>0</v>
+      </c>
       <c r="K66" s="3" t="e">
         <f>D66/SUM(C66:I66)</f>
         <v>#DIV/0!</v>
@@ -3952,8 +4725,27 @@
       <c r="B67" s="2">
         <v>2</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="E67" s="5"/>
+      <c r="C67" s="7">
+        <v>0</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0</v>
+      </c>
+      <c r="G67" s="7">
+        <v>0</v>
+      </c>
+      <c r="H67" s="7">
+        <v>0</v>
+      </c>
+      <c r="I67" s="7">
+        <v>0</v>
+      </c>
       <c r="K67" s="3" t="e">
         <f>E67/SUM(C67:I67)</f>
         <v>#DIV/0!</v>
@@ -3964,8 +4756,27 @@
       <c r="B68" s="2">
         <v>3</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="F68" s="5"/>
+      <c r="C68" s="7">
+        <v>0</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0</v>
+      </c>
+      <c r="G68" s="7">
+        <v>0</v>
+      </c>
+      <c r="H68" s="7">
+        <v>0</v>
+      </c>
+      <c r="I68" s="7">
+        <v>0</v>
+      </c>
       <c r="K68" s="3" t="e">
         <f>F68/SUM(C68:I68)</f>
         <v>#DIV/0!</v>
@@ -3978,8 +4789,27 @@
       <c r="B69" s="2">
         <v>4</v>
       </c>
-      <c r="C69" s="6"/>
-      <c r="G69" s="5"/>
+      <c r="C69" s="7">
+        <v>0</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7">
+        <v>0</v>
+      </c>
+      <c r="G69" s="7">
+        <v>0</v>
+      </c>
+      <c r="H69" s="7">
+        <v>0</v>
+      </c>
+      <c r="I69" s="7">
+        <v>0</v>
+      </c>
       <c r="K69" s="3" t="e">
         <f>G69/SUM(C69:I69)</f>
         <v>#DIV/0!</v>
@@ -3990,8 +4820,27 @@
       <c r="B70" s="2">
         <v>5</v>
       </c>
-      <c r="C70" s="6"/>
-      <c r="H70" s="5"/>
+      <c r="C70" s="7">
+        <v>0</v>
+      </c>
+      <c r="D70" s="7">
+        <v>0</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0</v>
+      </c>
+      <c r="F70" s="7">
+        <v>0</v>
+      </c>
+      <c r="G70" s="7">
+        <v>0</v>
+      </c>
+      <c r="H70" s="7">
+        <v>0</v>
+      </c>
+      <c r="I70" s="7">
+        <v>0</v>
+      </c>
       <c r="K70" s="3" t="e">
         <f>H70/SUM(C70:I70)</f>
         <v>#DIV/0!</v>
@@ -4002,8 +4851,27 @@
       <c r="B71" s="2">
         <v>6</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="I71" s="5"/>
+      <c r="C71" s="7">
+        <v>0</v>
+      </c>
+      <c r="D71" s="7">
+        <v>0</v>
+      </c>
+      <c r="E71" s="7">
+        <v>0</v>
+      </c>
+      <c r="F71" s="7">
+        <v>0</v>
+      </c>
+      <c r="G71" s="7">
+        <v>0</v>
+      </c>
+      <c r="H71" s="7">
+        <v>0</v>
+      </c>
+      <c r="I71" s="7">
+        <v>0</v>
+      </c>
       <c r="K71" s="3" t="e">
         <f>I71/SUM(C71:I71)</f>
         <v>#DIV/0!</v>

</xml_diff>